<commit_message>
Manutenção dos documentos do projeto para fase de elaboração
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C9663D-7092-4D4A-AFDF-245BCAC77426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="3000" yWindow="1995" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -14,7 +15,7 @@
     <sheet name="Ver-Construção1" sheetId="3" r:id="rId5"/>
     <sheet name="Ver-Transição1" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -202,12 +206,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -236,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -319,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -352,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -371,12 +375,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -405,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -488,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -521,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -540,12 +544,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -574,7 +578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -657,7 +661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -690,7 +694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -709,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="129">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1093,12 +1097,15 @@
   </si>
   <si>
     <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="16">
     <font>
       <sz val="11"/>
@@ -1561,7 +1568,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1637,7 +1644,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.92592592592592593</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1758,7 +1765,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2377,7 +2383,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2409,7 +2414,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2417,6 +2421,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2491,7 +2496,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2600,34 +2604,34 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2844,7 +2848,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2948,7 +2952,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2969,7 +2973,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3110,7 +3114,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3217,7 +3220,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3860,7 +3862,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3967,7 +3968,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4634,7 +4634,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7325,7 +7324,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7365,9 +7364,9 @@
       <c r="A4" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="20" t="e">
+      <c r="B4" s="20">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0.92592592592592593</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7401,7 +7400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -7475,21 +7474,21 @@
       <c r="N2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="26" t="e">
+      <c r="O2" s="26">
         <f>('Ver-Elaboração1'!$G$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P2" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P2" s="26">
         <f>('Ver-Elaboração1'!$H$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q2" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="26">
         <f>('Ver-Elaboração1'!$I$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R2" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R2" s="26">
         <f>('Ver-Elaboração1'!$J$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7515,21 +7514,21 @@
       <c r="N3" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="26" t="e">
+      <c r="O3" s="26">
         <f>('Ver-Elaboração1'!$G$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P3" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P3" s="26">
         <f>('Ver-Elaboração1'!$H$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q3" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="26">
         <f>('Ver-Elaboração1'!$I$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R3" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R3" s="26">
         <f>('Ver-Elaboração1'!$J$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -7555,21 +7554,21 @@
       <c r="N4" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="26" t="e">
+      <c r="O4" s="26">
         <f>('Ver-Elaboração1'!$G$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P4" s="26">
         <f>('Ver-Elaboração1'!$H$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q4" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="26">
         <f>('Ver-Elaboração1'!$I$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R4" s="26">
         <f>('Ver-Elaboração1'!$J$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -7595,21 +7594,21 @@
       <c r="N5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="26" t="e">
+      <c r="O5" s="26">
         <f>('Ver-Elaboração1'!$G$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="P5" s="26">
         <f>('Ver-Elaboração1'!$H$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q5" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="26">
         <f>('Ver-Elaboração1'!$I$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R5" s="26">
         <f>('Ver-Elaboração1'!$J$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -7635,21 +7634,21 @@
       <c r="N6" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="26" t="e">
+      <c r="O6" s="26">
         <f>('Ver-Elaboração1'!$G$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P6" s="26">
         <f>('Ver-Elaboração1'!$H$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q6" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="26">
         <f>('Ver-Elaboração1'!$I$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R6" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R6" s="26">
         <f>('Ver-Elaboração1'!$J$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -7675,21 +7674,21 @@
       <c r="N7" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="26" t="e">
+      <c r="O7" s="26">
         <f>('Ver-Elaboração1'!$G$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P7" s="26">
         <f>('Ver-Elaboração1'!$H$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="26">
         <f>('Ver-Elaboração1'!$I$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R7" s="26">
         <f>('Ver-Elaboração1'!$J$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -7715,21 +7714,21 @@
       <c r="N8" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="26" t="e">
+      <c r="O8" s="26">
         <f>('Ver-Elaboração1'!$G$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="P8" s="26">
         <f>('Ver-Elaboração1'!$H$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="26">
         <f>('Ver-Elaboração1'!$I$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="R8" s="26">
         <f>('Ver-Elaboração1'!$J$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -7755,21 +7754,21 @@
       <c r="N9" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="26" t="e">
+      <c r="O9" s="26">
         <f>('Ver-Elaboração1'!$G$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P9" s="26">
         <f>('Ver-Elaboração1'!$H$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="26">
         <f>('Ver-Elaboração1'!$I$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R9" s="26">
         <f>('Ver-Elaboração1'!$J$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -7795,21 +7794,21 @@
       <c r="N10" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="26" t="e">
+      <c r="O10" s="26">
         <f>('Ver-Elaboração1'!$G$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P10" s="26">
         <f>('Ver-Elaboração1'!$H$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="26">
         <f>('Ver-Elaboração1'!$I$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R10" s="26">
         <f>('Ver-Elaboração1'!$J$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -7835,21 +7834,21 @@
       <c r="N11" t="s">
         <v>70</v>
       </c>
-      <c r="O11" s="26" t="e">
+      <c r="O11" s="26">
         <f>('Ver-Elaboração1'!$G$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="26" t="e">
+        <v>1</v>
+      </c>
+      <c r="P11" s="26">
         <f>('Ver-Elaboração1'!$H$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="26">
         <f>('Ver-Elaboração1'!$I$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R11" s="26">
         <f>('Ver-Elaboração1'!$J$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -7875,21 +7874,21 @@
       <c r="N12" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="26" t="e">
+      <c r="O12" s="26">
         <f>('Ver-Elaboração1'!$G$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="P12" s="26">
         <f>('Ver-Elaboração1'!$H$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="26">
         <f>('Ver-Elaboração1'!$I$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="26" t="e">
+        <v>0</v>
+      </c>
+      <c r="R12" s="26">
         <f>('Ver-Elaboração1'!$J$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -8439,10 +8438,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -9341,10 +9340,10 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D29 D31:D33 D45:D48 D50:D52 D14:D18 D8:D12 D35:D43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D29 D31:D33 D45:D48 D50:D52 D14:D18 D8:D12 D35:D43" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9355,11 +9354,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9393,9 +9392,9 @@
         <v>46</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="21" t="e">
+      <c r="F2" s="21">
         <f>COUNTIF(D5:D48,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.92592592592592593</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1">
@@ -9450,12 +9449,14 @@
       <c r="C6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -9488,12 +9489,14 @@
       <c r="C8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -9526,12 +9529,14 @@
       <c r="C10" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10">
         <f>COUNTIF(D10:D13,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <f>COUNTIF(D10:D13,"Parcialmente")</f>
@@ -9554,7 +9559,9 @@
       <c r="C11" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
@@ -9566,7 +9573,9 @@
       <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -9578,7 +9587,9 @@
       <c r="C13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
@@ -9600,7 +9611,9 @@
       <c r="C15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15">
@@ -9617,7 +9630,7 @@
       </c>
       <c r="J15">
         <f>COUNTIF(D15,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15">
@@ -9638,12 +9651,14 @@
       <c r="C17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17">
         <f>COUNTIF(D17,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <f>COUNTIF(D17,"Parcialmente")</f>
@@ -9678,12 +9693,14 @@
       <c r="C19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19">
         <f>COUNTIF(D19:D23,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19">
         <f>COUNTIF(D19:D23,"Parcialmente")</f>
@@ -9718,7 +9735,9 @@
       <c r="C21" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -9742,7 +9761,9 @@
       <c r="C23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
@@ -9764,7 +9785,9 @@
       <c r="C25" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25">
@@ -9777,7 +9800,7 @@
       </c>
       <c r="I25">
         <f>COUNTIF(D25:D26,"Não")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25">
         <f>COUNTIF(D25:D26,"NA")</f>
@@ -9792,7 +9815,9 @@
       <c r="C26" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
@@ -9816,12 +9841,14 @@
       <c r="C28" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28">
         <f>COUNTIF(D28:D33,"Sim")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H28">
         <f>COUNTIF(D28:D33,"Parcialmente")</f>
@@ -9844,7 +9871,9 @@
       <c r="C29" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
@@ -9856,7 +9885,9 @@
       <c r="C30" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
@@ -9868,7 +9899,9 @@
       <c r="C31" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -9880,7 +9913,9 @@
       <c r="C32" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
@@ -9892,7 +9927,9 @@
       <c r="C33" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
@@ -9916,12 +9953,14 @@
       <c r="C35" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35">
         <f>COUNTIF(D35:D40,"Sim")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H35">
         <f>COUNTIF(D35:D40,"Parcialmente")</f>
@@ -9944,7 +9983,9 @@
       <c r="C36" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
@@ -9956,7 +9997,9 @@
       <c r="C37" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
@@ -9968,7 +10011,9 @@
       <c r="C38" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -9980,7 +10025,9 @@
       <c r="C39" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
@@ -9992,7 +10039,9 @@
       <c r="C40" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
@@ -10016,12 +10065,14 @@
       <c r="C42" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42">
         <f>COUNTIF(D42:D44,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H42">
         <f>COUNTIF(D42:D44,"Parcialmente")</f>
@@ -10044,7 +10095,9 @@
       <c r="C43" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
@@ -10056,7 +10109,9 @@
       <c r="C44" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
@@ -10078,7 +10133,9 @@
       <c r="C46" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46">
@@ -10095,7 +10152,7 @@
       </c>
       <c r="J46">
         <f>COUNTIF(D46:D48,"NA")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15">
@@ -10106,7 +10163,9 @@
       <c r="C47" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
@@ -10118,7 +10177,9 @@
       <c r="C48" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
@@ -10136,10 +10197,10 @@
     <mergeCell ref="A5:A17"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18 D24 D27 D34 D41 D45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18 D24 D27 D34 D41 D45" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46:D48 D42:D44 D35:D40 D28:D33 D25:D26 D19:D23 D17 D15 D10:D13 D8 D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46:D48 D42:D44 D35:D40 D28:D33 D25:D26 D19:D23 D17 D15 D10:D13 D8 D6" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10149,7 +10210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -10998,23 +11059,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D18:D19 D21 D23:D28 D30:D36 D38:D43 D45:D47 D49:D51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D18:D19 D21 D23:D28 D30:D36 D38:D43 D45:D47 D49:D51" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11024,7 +11085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -11877,6 +11938,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -11884,17 +11950,12 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D18 D20:D24 D26:D28 D30:D31 D33:D34 D36:D42 D44:D46 D48:D50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D18 D20:D24 D26:D28 D30:D31 D33:D34 D36:D42 D44:D46 D48:D50" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Adição do Guia de Implementação
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C9663D-7092-4D4A-AFDF-245BCAC77426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE3E06-CBBA-4EA1-926F-3E4AA11FAD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1995" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -713,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="128">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1097,9 +1097,6 @@
   </si>
   <si>
     <t>Sim</t>
-  </si>
-  <si>
-    <t>Não</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1641,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92592592592592593</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2622,7 +2619,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -2848,7 +2845,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -7366,7 +7363,7 @@
       </c>
       <c r="B4" s="20">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.92592592592592593</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7716,7 +7713,7 @@
       </c>
       <c r="O8" s="26">
         <f>('Ver-Elaboração1'!$G$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="26">
         <f>('Ver-Elaboração1'!$H$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
@@ -7724,7 +7721,7 @@
       </c>
       <c r="Q8" s="26">
         <f>('Ver-Elaboração1'!$I$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="26">
         <f>('Ver-Elaboração1'!$J$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
@@ -9357,8 +9354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9394,7 +9391,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D48,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>0.92592592592592593</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1">
@@ -9700,7 +9697,7 @@
       <c r="F19" s="8"/>
       <c r="G19">
         <f>COUNTIF(D19:D23,"Sim")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f>COUNTIF(D19:D23,"Parcialmente")</f>
@@ -9749,7 +9746,9 @@
       <c r="C22" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
@@ -9786,13 +9785,13 @@
         <v>98</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25">
         <f>COUNTIF(D25:D26,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <f>COUNTIF(D25:D26,"Parcialmente")</f>
@@ -9800,7 +9799,7 @@
       </c>
       <c r="I25">
         <f>COUNTIF(D25:D26,"Não")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <f>COUNTIF(D25:D26,"NA")</f>
@@ -9816,7 +9815,7 @@
         <v>60</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -11059,17 +11058,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11938,11 +11937,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -11950,6 +11944,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
Adição do Modelo de Deployment e do Modelo de Arquitetura do Frontend
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE3E06-CBBA-4EA1-926F-3E4AA11FAD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC2961C-2E65-4632-B23B-F48D0A3BE9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -713,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="128">
   <si>
     <t>Ambiente</t>
   </si>
@@ -9355,7 +9355,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9697,7 +9697,7 @@
       <c r="F19" s="8"/>
       <c r="G19">
         <f>COUNTIF(D19:D23,"Sim")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H19">
         <f>COUNTIF(D19:D23,"Parcialmente")</f>
@@ -9720,7 +9720,9 @@
       <c r="C20" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -11058,17 +11060,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11937,6 +11939,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -11944,11 +11951,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
Modificação nos códigos para deploy na AWS
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC2961C-2E65-4632-B23B-F48D0A3BE9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3860E394-7B06-4978-A0B1-C2E3BEBB8F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -713,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="128">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1644,7 +1644,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3328,10 +3328,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3691,10 +3691,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -7370,9 +7370,9 @@
       <c r="A5" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="20" t="e">
+      <c r="B5" s="20">
         <f>'Ver-Construção1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7909,42 +7909,42 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="27" t="e">
+      <c r="B23" s="27">
         <f>('Ver-Construção1'!$G$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C23" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="C23" s="28">
         <f>('Ver-Construção1'!$H$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D23" s="28">
         <f>('Ver-Construção1'!$I$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E23" s="28">
         <f>('Ver-Construção1'!$J$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="27" t="e">
+      <c r="B24" s="27">
         <f>('Ver-Construção1'!$G$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="C24" s="28">
         <f>('Ver-Construção1'!$H$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D24" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D24" s="28">
         <f>('Ver-Construção1'!$I$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E24" s="28">
         <f>('Ver-Construção1'!$J$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M24" t="s">
         <v>121</v>
@@ -7966,21 +7966,21 @@
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="27" t="e">
+      <c r="B25" s="27">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C25" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="C25" s="28">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D25" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D25" s="28">
         <f>('Ver-Construção1'!$I$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E25" s="28">
         <f>('Ver-Construção1'!$J$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M25" t="s">
         <v>2</v>
@@ -8006,21 +8006,21 @@
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="28" t="e">
+      <c r="B26" s="28">
         <f>('Ver-Construção1'!$G$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C26" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="C26" s="28">
         <f>('Ver-Construção1'!$H$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D26" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D26" s="28">
         <f>('Ver-Construção1'!$I$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E26" s="28">
         <f>('Ver-Construção1'!$J$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M26" t="s">
         <v>3</v>
@@ -9354,7 +9354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B24" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -10214,8 +10214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -10249,9 +10249,9 @@
         <v>46</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="21" t="e">
+      <c r="F2" s="21">
         <f>COUNTIF(D5:D51,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1">
@@ -10306,12 +10306,14 @@
       <c r="C6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -10344,12 +10346,14 @@
       <c r="C8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -10382,7 +10386,9 @@
       <c r="C10" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10">
@@ -10399,7 +10405,7 @@
       </c>
       <c r="J10">
         <f>COUNTIF(D10:D12,"NA")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
@@ -10410,7 +10416,9 @@
       <c r="C11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
@@ -10422,7 +10430,9 @@
       <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -10444,7 +10454,9 @@
       <c r="C14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14">
@@ -10461,7 +10473,7 @@
       </c>
       <c r="J14">
         <f>COUNTIF(D14,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15">
@@ -11060,17 +11072,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11939,11 +11951,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -11951,6 +11958,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
Adição da documentação da fase de construção
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3860E394-7B06-4978-A0B1-C2E3BEBB8F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832DD8BB-D6D5-4CB2-A84B-4BC41AFEE61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -713,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="128">
   <si>
     <t>Ambiente</t>
   </si>
@@ -3340,25 +3340,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3703,22 +3703,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.42857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7328,13 +7328,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:2" ht="18">
       <c r="A1" s="29" t="s">
         <v>96</v>
       </c>
@@ -7404,16 +7404,16 @@
       <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -8046,21 +8046,21 @@
       <c r="A27" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="28" t="e">
+      <c r="B27" s="28">
         <f>('Ver-Construção1'!$G$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C27" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="C27" s="28">
         <f>('Ver-Construção1'!$H$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D27" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D27" s="28">
         <f>('Ver-Construção1'!$I$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E27" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E27" s="28">
         <f>('Ver-Construção1'!$J$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M27" t="s">
         <v>14</v>
@@ -8086,21 +8086,21 @@
       <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="28" t="e">
+      <c r="B28" s="28">
         <f>('Ver-Construção1'!$G$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="C28" s="28">
         <f>('Ver-Construção1'!$H$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D28" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D28" s="28">
         <f>('Ver-Construção1'!$I$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E28" s="28">
         <f>('Ver-Construção1'!$J$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M28" t="s">
         <v>4</v>
@@ -8126,21 +8126,21 @@
       <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="28" t="e">
+      <c r="B29" s="28">
         <f>('Ver-Construção1'!$G$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C29" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="C29" s="28">
         <f>('Ver-Construção1'!$H$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D29" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D29" s="28">
         <f>('Ver-Construção1'!$I$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E29" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E29" s="28">
         <f>('Ver-Construção1'!$J$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M29" t="s">
         <v>36</v>
@@ -8166,21 +8166,21 @@
       <c r="A30" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="28" t="e">
+      <c r="B30" s="28">
         <f>('Ver-Construção1'!$G$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C30" s="28" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="28">
         <f>('Ver-Construção1'!$H$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D30" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D30" s="28">
         <f>('Ver-Construção1'!$I$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E30" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E30" s="28">
         <f>('Ver-Construção1'!$J$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="M30" t="s">
         <v>5</v>
@@ -8206,21 +8206,21 @@
       <c r="A31" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="28" t="e">
+      <c r="B31" s="28">
         <f>('Ver-Construção1'!$G$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C31" s="28" t="e">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="C31" s="28">
         <f>('Ver-Construção1'!$H$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D31" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D31" s="28">
         <f>('Ver-Construção1'!$I$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E31" s="28">
         <f>('Ver-Construção1'!$J$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="M31" t="s">
         <v>6</v>
@@ -8246,21 +8246,21 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="28" t="e">
+      <c r="B32" s="28">
         <f>('Ver-Construção1'!$G$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C32" s="28" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C32" s="28">
         <f>('Ver-Construção1'!$H$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D32" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D32" s="28">
         <f>('Ver-Construção1'!$I$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E32" s="28">
         <f>('Ver-Construção1'!$J$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M32" t="s">
         <v>8</v>
@@ -8286,21 +8286,21 @@
       <c r="A33" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="28" t="e">
+      <c r="B33" s="28">
         <f>('Ver-Construção1'!$G$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="C33" s="28">
         <f>('Ver-Construção1'!$H$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D33" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D33" s="28">
         <f>('Ver-Construção1'!$I$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E33" s="28">
         <f>('Ver-Construção1'!$J$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M33" t="s">
         <v>9</v>
@@ -8326,21 +8326,21 @@
       <c r="A34" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="28" t="e">
+      <c r="B34" s="28">
         <f>('Ver-Construção1'!$G$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C34" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="C34" s="28">
         <f>('Ver-Construção1'!$H$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="D34" s="28">
         <f>('Ver-Construção1'!$I$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="E34" s="28">
         <f>('Ver-Construção1'!$J$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M34" t="s">
         <v>10</v>
@@ -8442,17 +8442,17 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="91" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="4.42578125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="6" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8481,7 +8481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5" thickBot="1">
+    <row r="3" spans="1:10" ht="16.2" thickBot="1">
       <c r="A3" s="35" t="s">
         <v>26</v>
       </c>
@@ -8493,7 +8493,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="39"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" ht="14.4">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10" ht="14.4">
       <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
@@ -8541,7 +8541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10" ht="14.4">
       <c r="A6" s="36"/>
       <c r="B6" s="5">
         <v>1</v>
@@ -8597,7 +8597,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10" ht="14.4">
       <c r="A9" s="33"/>
       <c r="B9" s="5">
         <v>3</v>
@@ -8611,7 +8611,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10" ht="14.4">
       <c r="A10" s="33"/>
       <c r="B10" s="5">
         <v>4</v>
@@ -8625,7 +8625,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="14.4">
       <c r="A11" s="33"/>
       <c r="B11" s="5">
         <v>5</v>
@@ -8653,7 +8653,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10" ht="14.4">
       <c r="A13" s="33"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
@@ -8679,7 +8679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" ht="14.4">
       <c r="A14" s="33"/>
       <c r="B14" s="23">
         <v>7</v>
@@ -8693,7 +8693,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A15" s="33"/>
       <c r="B15" s="5">
         <v>8</v>
@@ -8707,7 +8707,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A16" s="33"/>
       <c r="B16" s="5">
         <v>9</v>
@@ -8721,7 +8721,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="15">
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="14.4">
       <c r="A17" s="33"/>
       <c r="B17" s="23">
         <v>10</v>
@@ -8735,7 +8735,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="15">
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="14.4">
       <c r="A18" s="33"/>
       <c r="B18" s="5">
         <v>11</v>
@@ -8749,7 +8749,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:10" ht="14.4">
       <c r="A19" s="33"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
@@ -8775,7 +8775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30">
+    <row r="20" spans="1:10" ht="14.4">
       <c r="A20" s="33"/>
       <c r="B20" s="23">
         <v>12</v>
@@ -8789,7 +8789,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="30">
+    <row r="21" spans="1:10" ht="28.8">
       <c r="A21" s="33"/>
       <c r="B21" s="5">
         <v>13</v>
@@ -8803,7 +8803,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15">
+    <row r="22" spans="1:10" ht="14.4">
       <c r="A22" s="33"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
@@ -8829,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10" ht="14.4">
       <c r="A23" s="33"/>
       <c r="B23" s="23">
         <v>14</v>
@@ -8843,7 +8843,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="15">
+    <row r="24" spans="1:10" ht="14.4">
       <c r="A24" s="33"/>
       <c r="B24" s="5">
         <v>15</v>
@@ -8857,7 +8857,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10" ht="14.4">
       <c r="A25" s="33"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
@@ -8883,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15">
+    <row r="26" spans="1:10" ht="14.4">
       <c r="A26" s="33"/>
       <c r="B26" s="23">
         <v>16</v>
@@ -8897,7 +8897,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="15">
+    <row r="27" spans="1:10" ht="14.4">
       <c r="A27" s="33"/>
       <c r="B27" s="5">
         <v>17</v>
@@ -8911,7 +8911,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="15">
+    <row r="28" spans="1:10" ht="14.4">
       <c r="A28" s="32" t="s">
         <v>11</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15">
+    <row r="29" spans="1:10" ht="14.4">
       <c r="A29" s="33"/>
       <c r="B29" s="23">
         <v>18</v>
@@ -8953,7 +8953,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:10" ht="15">
+    <row r="30" spans="1:10" ht="14.4">
       <c r="A30" s="33"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10" t="s">
@@ -8979,7 +8979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15">
+    <row r="31" spans="1:10" ht="14.4">
       <c r="A31" s="33"/>
       <c r="B31" s="23">
         <v>18</v>
@@ -8993,7 +8993,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="15">
+    <row r="32" spans="1:10" ht="14.4">
       <c r="A32" s="33"/>
       <c r="B32" s="5">
         <v>19</v>
@@ -9007,7 +9007,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="15">
+    <row r="33" spans="1:10" ht="14.4">
       <c r="A33" s="33"/>
       <c r="B33" s="5">
         <v>20</v>
@@ -9021,7 +9021,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="15">
+    <row r="34" spans="1:10" ht="14.4">
       <c r="A34" s="33"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10" t="s">
@@ -9047,7 +9047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15">
+    <row r="35" spans="1:10" ht="14.4">
       <c r="A35" s="33"/>
       <c r="B35" s="23">
         <v>21</v>
@@ -9061,7 +9061,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:10" ht="14.4">
       <c r="A36" s="33"/>
       <c r="B36" s="5">
         <v>22</v>
@@ -9075,7 +9075,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:10" ht="15">
+    <row r="37" spans="1:10" ht="14.4">
       <c r="A37" s="33"/>
       <c r="B37" s="5">
         <v>23</v>
@@ -9089,7 +9089,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="15">
+    <row r="38" spans="1:10" ht="14.4">
       <c r="A38" s="33"/>
       <c r="B38" s="5">
         <v>24</v>
@@ -9103,7 +9103,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="15">
+    <row r="39" spans="1:10" ht="14.4">
       <c r="A39" s="33"/>
       <c r="B39" s="5">
         <v>25</v>
@@ -9117,7 +9117,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="15">
+    <row r="40" spans="1:10" ht="14.4">
       <c r="A40" s="33"/>
       <c r="B40" s="5">
         <v>26</v>
@@ -9144,7 +9144,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:10" ht="15">
+    <row r="42" spans="1:10" ht="14.4">
       <c r="A42" s="33"/>
       <c r="B42" s="5">
         <v>28</v>
@@ -9158,7 +9158,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:10" ht="15">
+    <row r="43" spans="1:10" ht="14.4">
       <c r="A43" s="24"/>
       <c r="B43" s="5">
         <v>29</v>
@@ -9200,7 +9200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="30">
+    <row r="45" spans="1:10" ht="14.4">
       <c r="A45" s="31"/>
       <c r="B45" s="23">
         <v>30</v>
@@ -9214,7 +9214,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:10" ht="15">
+    <row r="46" spans="1:10" ht="14.4">
       <c r="A46" s="31"/>
       <c r="B46" s="5">
         <v>31</v>
@@ -9228,7 +9228,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:10" ht="15">
+    <row r="47" spans="1:10" ht="14.4">
       <c r="A47" s="31"/>
       <c r="B47" s="5">
         <v>32</v>
@@ -9256,7 +9256,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:10" ht="15">
+    <row r="49" spans="1:10" ht="14.4">
       <c r="A49" s="31"/>
       <c r="B49" s="9"/>
       <c r="C49" s="10" t="s">
@@ -9282,7 +9282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15">
+    <row r="50" spans="1:10" ht="14.4">
       <c r="A50" s="31"/>
       <c r="B50" s="23">
         <v>34</v>
@@ -9296,7 +9296,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:10" ht="15">
+    <row r="51" spans="1:10" ht="14.4">
       <c r="A51" s="31"/>
       <c r="B51" s="5">
         <v>35</v>
@@ -9310,7 +9310,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:10" ht="15">
+    <row r="52" spans="1:10" ht="14.4">
       <c r="A52" s="31"/>
       <c r="B52" s="5">
         <v>36</v>
@@ -9358,14 +9358,14 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="68" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
     <col min="7" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9394,7 +9394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5" thickBot="1">
+    <row r="3" spans="1:10" ht="16.2" thickBot="1">
       <c r="A3" s="35" t="s">
         <v>26</v>
       </c>
@@ -9406,7 +9406,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="39"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" ht="14.4">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -9438,7 +9438,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="28.8">
       <c r="A6" s="33"/>
       <c r="B6" s="5">
         <v>1</v>
@@ -9468,7 +9468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" ht="14.4">
       <c r="A7" s="33"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
@@ -9478,7 +9478,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A8" s="33"/>
       <c r="B8" s="5">
         <v>2</v>
@@ -9508,7 +9508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10" ht="14.4">
       <c r="A9" s="33"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
@@ -9518,7 +9518,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="45">
+    <row r="10" spans="1:10" ht="43.2">
       <c r="A10" s="33"/>
       <c r="B10" s="23">
         <v>3</v>
@@ -9548,7 +9548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30">
+    <row r="11" spans="1:10" ht="28.8">
       <c r="A11" s="33"/>
       <c r="B11" s="23">
         <v>4</v>
@@ -9562,7 +9562,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="30">
+    <row r="12" spans="1:10" ht="14.4">
       <c r="A12" s="33"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -9576,7 +9576,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="30">
+    <row r="13" spans="1:10" ht="28.8">
       <c r="A13" s="33"/>
       <c r="B13" s="5">
         <v>6</v>
@@ -9590,7 +9590,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" ht="14.4">
       <c r="A14" s="33"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
@@ -9600,7 +9600,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" ht="14.4">
       <c r="A15" s="33"/>
       <c r="B15" s="5">
         <v>7</v>
@@ -9630,7 +9630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10" ht="14.4">
       <c r="A16" s="33"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10" t="s">
@@ -9640,7 +9640,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10" ht="14.4">
       <c r="A17" s="33"/>
       <c r="B17" s="5">
         <v>8</v>
@@ -9682,7 +9682,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:10" ht="30">
+    <row r="19" spans="1:10" ht="28.8">
       <c r="A19" s="33"/>
       <c r="B19" s="5">
         <v>9</v>
@@ -9712,7 +9712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30">
+    <row r="20" spans="1:10" ht="28.8">
       <c r="A20" s="33"/>
       <c r="B20" s="23">
         <v>10</v>
@@ -9726,7 +9726,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A21" s="33"/>
       <c r="B21" s="5">
         <v>11</v>
@@ -9740,7 +9740,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="45">
+    <row r="22" spans="1:10" ht="28.8">
       <c r="A22" s="33"/>
       <c r="B22" s="5">
         <v>12</v>
@@ -9754,7 +9754,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="30">
+    <row r="23" spans="1:10" ht="28.8">
       <c r="A23" s="33"/>
       <c r="B23" s="5">
         <v>13</v>
@@ -9768,7 +9768,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="15">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="14.4">
       <c r="A24" s="33"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
@@ -9778,7 +9778,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="25" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A25" s="33"/>
       <c r="B25" s="23">
         <v>15</v>
@@ -9808,7 +9808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A26" s="33"/>
       <c r="B26" s="5">
         <v>16</v>
@@ -9822,7 +9822,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="15">
+    <row r="27" spans="1:10" ht="14.4">
       <c r="A27" s="32" t="s">
         <v>19</v>
       </c>
@@ -9834,7 +9834,7 @@
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:10" ht="30">
+    <row r="28" spans="1:10" ht="28.8">
       <c r="A28" s="33"/>
       <c r="B28" s="5">
         <v>17</v>
@@ -9864,7 +9864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30">
+    <row r="29" spans="1:10" ht="28.8">
       <c r="A29" s="33"/>
       <c r="B29" s="5">
         <v>18</v>
@@ -9878,7 +9878,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:10" ht="30">
+    <row r="30" spans="1:10" ht="14.4">
       <c r="A30" s="33"/>
       <c r="B30" s="5">
         <v>19</v>
@@ -9892,7 +9892,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:10" ht="15">
+    <row r="31" spans="1:10" ht="14.4">
       <c r="A31" s="33"/>
       <c r="B31" s="23">
         <v>20</v>
@@ -9906,7 +9906,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="30">
+    <row r="32" spans="1:10" ht="28.8">
       <c r="A32" s="33"/>
       <c r="B32" s="5">
         <v>21</v>
@@ -9920,7 +9920,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="15">
+    <row r="33" spans="1:10" ht="14.4">
       <c r="A33" s="33"/>
       <c r="B33" s="5">
         <v>22</v>
@@ -9934,7 +9934,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="15">
+    <row r="34" spans="1:10" ht="14.4">
       <c r="A34" s="42" t="s">
         <v>11</v>
       </c>
@@ -9946,7 +9946,7 @@
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:10" ht="15">
+    <row r="35" spans="1:10" ht="14.4">
       <c r="A35" s="42"/>
       <c r="B35" s="5">
         <v>23</v>
@@ -9976,7 +9976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:10" ht="14.4">
       <c r="A36" s="42"/>
       <c r="B36" s="5">
         <v>24</v>
@@ -9990,7 +9990,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:10" ht="30">
+    <row r="37" spans="1:10" ht="28.8">
       <c r="A37" s="42"/>
       <c r="B37" s="5">
         <v>25</v>
@@ -10004,7 +10004,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="15">
+    <row r="38" spans="1:10" ht="14.4">
       <c r="A38" s="42"/>
       <c r="B38" s="5">
         <v>26</v>
@@ -10018,7 +10018,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="15">
+    <row r="39" spans="1:10" ht="14.4">
       <c r="A39" s="42"/>
       <c r="B39" s="5">
         <v>27</v>
@@ -10032,7 +10032,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="15">
+    <row r="40" spans="1:10" ht="14.4">
       <c r="A40" s="42"/>
       <c r="B40" s="5">
         <v>28</v>
@@ -10058,7 +10058,7 @@
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:10" ht="30">
+    <row r="42" spans="1:10" ht="28.8">
       <c r="A42" s="31"/>
       <c r="B42" s="5">
         <v>29</v>
@@ -10088,7 +10088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15">
+    <row r="43" spans="1:10" ht="14.4">
       <c r="A43" s="31"/>
       <c r="B43" s="5">
         <v>30</v>
@@ -10102,7 +10102,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:10" ht="30">
+    <row r="44" spans="1:10" ht="28.8">
       <c r="A44" s="31"/>
       <c r="B44" s="5">
         <v>31</v>
@@ -10116,7 +10116,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:10" ht="15">
+    <row r="45" spans="1:10" ht="14.4">
       <c r="A45" s="31"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10" t="s">
@@ -10126,7 +10126,7 @@
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
     </row>
-    <row r="46" spans="1:10" ht="30">
+    <row r="46" spans="1:10" ht="28.8">
       <c r="A46" s="31"/>
       <c r="B46" s="5">
         <v>32</v>
@@ -10156,7 +10156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15">
+    <row r="47" spans="1:10" ht="14.4">
       <c r="A47" s="31"/>
       <c r="B47" s="5">
         <v>33</v>
@@ -10170,7 +10170,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:10" ht="15">
+    <row r="48" spans="1:10" ht="14.4">
       <c r="A48" s="31"/>
       <c r="B48" s="5">
         <v>34</v>
@@ -10214,19 +10214,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="71.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
@@ -10254,7 +10254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5" thickBot="1">
+    <row r="3" spans="1:10" ht="16.2" thickBot="1">
       <c r="A3" s="35" t="s">
         <v>26</v>
       </c>
@@ -10266,7 +10266,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="39"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" ht="14.4">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -10298,7 +10298,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="28.8">
       <c r="A6" s="33"/>
       <c r="B6" s="5">
         <v>1</v>
@@ -10328,7 +10328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" ht="14.4">
       <c r="A7" s="33"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
@@ -10338,7 +10338,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A8" s="33"/>
       <c r="B8" s="5">
         <v>2</v>
@@ -10368,7 +10368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10" ht="14.4">
       <c r="A9" s="33"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
@@ -10378,7 +10378,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="45">
+    <row r="10" spans="1:10" ht="43.2">
       <c r="A10" s="33"/>
       <c r="B10" s="5">
         <v>3</v>
@@ -10408,7 +10408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30">
+    <row r="11" spans="1:10" ht="28.8">
       <c r="A11" s="33"/>
       <c r="B11" s="5">
         <v>4</v>
@@ -10436,7 +10436,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10" ht="14.4">
       <c r="A13" s="33"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
@@ -10446,7 +10446,7 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" ht="14.4">
       <c r="A14" s="33"/>
       <c r="B14" s="5">
         <v>6</v>
@@ -10476,7 +10476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" ht="14.4">
       <c r="A15" s="33"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
@@ -10486,7 +10486,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10" ht="14.4">
       <c r="A16" s="33"/>
       <c r="B16" s="5">
         <v>7</v>
@@ -10494,12 +10494,14 @@
       <c r="C16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
         <f>COUNTIF(D16,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <f>COUNTIF(D16,"Parcialmente")</f>
@@ -10526,7 +10528,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10" ht="14.4">
       <c r="A18" s="33"/>
       <c r="B18" s="5">
         <v>8</v>
@@ -10534,12 +10536,14 @@
       <c r="C18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18">
         <f>COUNTIF(D18:D19,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <f>COUNTIF(D18:D19,"Parcialmente")</f>
@@ -10554,7 +10558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30">
+    <row r="19" spans="1:10" ht="28.8">
       <c r="A19" s="33"/>
       <c r="B19" s="5">
         <v>9</v>
@@ -10562,11 +10566,13 @@
       <c r="C19" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="15">
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="14.4">
       <c r="A20" s="33"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
@@ -10576,7 +10582,7 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A21" s="33"/>
       <c r="B21" s="5">
         <v>10</v>
@@ -10584,7 +10590,9 @@
       <c r="C21" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21">
@@ -10601,10 +10609,10 @@
       </c>
       <c r="J21">
         <f>COUNTIF(D21,"NA")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.4">
       <c r="A22" s="32" t="s">
         <v>19</v>
       </c>
@@ -10616,7 +10624,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:10" ht="45">
+    <row r="23" spans="1:10" ht="43.2">
       <c r="A23" s="33"/>
       <c r="B23" s="5">
         <v>11</v>
@@ -10624,12 +10632,14 @@
       <c r="C23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23">
         <f>COUNTIF(D23:D28,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H23">
         <f>COUNTIF(D23:D28,"Parcialmente")</f>
@@ -10641,10 +10651,10 @@
       </c>
       <c r="J23">
         <f>COUNTIF(D23:D28,"NA")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="28.8">
       <c r="A24" s="33"/>
       <c r="B24" s="5">
         <v>12</v>
@@ -10652,11 +10662,13 @@
       <c r="C24" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="30">
+    <row r="25" spans="1:10" ht="14.4">
       <c r="A25" s="33"/>
       <c r="B25" s="5">
         <v>13</v>
@@ -10664,11 +10676,13 @@
       <c r="C25" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="15">
+    <row r="26" spans="1:10" ht="14.4">
       <c r="A26" s="33"/>
       <c r="B26" s="5">
         <v>14</v>
@@ -10676,11 +10690,13 @@
       <c r="C26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10" ht="28.8">
       <c r="A27" s="33"/>
       <c r="B27" s="5">
         <v>15</v>
@@ -10688,11 +10704,13 @@
       <c r="C27" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="15">
+    <row r="28" spans="1:10" ht="14.4">
       <c r="A28" s="33"/>
       <c r="B28" s="5">
         <v>16</v>
@@ -10700,11 +10718,13 @@
       <c r="C28" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:10" ht="15">
+    <row r="29" spans="1:10" ht="14.4">
       <c r="A29" s="32" t="s">
         <v>20</v>
       </c>
@@ -10716,7 +10736,7 @@
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:10" ht="30">
+    <row r="30" spans="1:10" ht="28.8">
       <c r="A30" s="33"/>
       <c r="B30" s="23">
         <v>17</v>
@@ -10724,12 +10744,14 @@
       <c r="C30" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30">
         <f>COUNTIF(D30:D36,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <f>COUNTIF(D30:D36,"Parcialmente")</f>
@@ -10741,10 +10763,10 @@
       </c>
       <c r="J30">
         <f>COUNTIF(D30:D36,"NA")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="28.8">
       <c r="A31" s="33"/>
       <c r="B31" s="5">
         <v>18</v>
@@ -10752,11 +10774,13 @@
       <c r="C31" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="15">
+    <row r="32" spans="1:10" ht="14.4">
       <c r="A32" s="33"/>
       <c r="B32" s="5">
         <v>19</v>
@@ -10764,11 +10788,13 @@
       <c r="C32" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="15">
+    <row r="33" spans="1:10" ht="14.4">
       <c r="A33" s="33"/>
       <c r="B33" s="5">
         <v>20</v>
@@ -10776,11 +10802,13 @@
       <c r="C33" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="15">
+    <row r="34" spans="1:10" ht="14.4">
       <c r="A34" s="33"/>
       <c r="B34" s="5">
         <v>21</v>
@@ -10788,11 +10816,13 @@
       <c r="C34" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="30">
+    <row r="35" spans="1:10" ht="14.4">
       <c r="A35" s="33"/>
       <c r="B35" s="5">
         <v>22</v>
@@ -10800,11 +10830,13 @@
       <c r="C35" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:10" ht="14.4">
       <c r="A36" s="36"/>
       <c r="B36" s="5">
         <v>23</v>
@@ -10812,11 +10844,13 @@
       <c r="C36" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:10" ht="15">
+    <row r="37" spans="1:10" ht="14.4">
       <c r="A37" s="42" t="s">
         <v>11</v>
       </c>
@@ -10828,7 +10862,7 @@
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:10" ht="30">
+    <row r="38" spans="1:10" ht="28.8">
       <c r="A38" s="42"/>
       <c r="B38" s="5">
         <v>24</v>
@@ -10836,12 +10870,14 @@
       <c r="C38" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38">
         <f>COUNTIF(D38:D43,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H38">
         <f>COUNTIF(D38:D43,"Parcialmente")</f>
@@ -10853,10 +10889,10 @@
       </c>
       <c r="J38">
         <f>COUNTIF(D38:D43,"NA")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="43.2">
       <c r="A39" s="42"/>
       <c r="B39" s="5">
         <v>25</v>
@@ -10864,11 +10900,13 @@
       <c r="C39" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="30">
+    <row r="40" spans="1:10" ht="14.4">
       <c r="A40" s="42"/>
       <c r="B40" s="5">
         <v>26</v>
@@ -10876,11 +10914,13 @@
       <c r="C40" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="15">
+    <row r="41" spans="1:10" ht="14.4">
       <c r="A41" s="42"/>
       <c r="B41" s="5">
         <v>27</v>
@@ -10888,11 +10928,13 @@
       <c r="C41" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:10" ht="15">
+    <row r="42" spans="1:10" ht="14.4">
       <c r="A42" s="42"/>
       <c r="B42" s="5">
         <v>28</v>
@@ -10900,11 +10942,13 @@
       <c r="C42" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:10" ht="15">
+    <row r="43" spans="1:10" ht="14.4">
       <c r="A43" s="42"/>
       <c r="B43" s="5">
         <v>29</v>
@@ -10912,7 +10956,9 @@
       <c r="C43" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
@@ -10928,7 +10974,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:10" ht="30">
+    <row r="45" spans="1:10" ht="28.8">
       <c r="A45" s="31"/>
       <c r="B45" s="5">
         <v>30</v>
@@ -10936,12 +10982,14 @@
       <c r="C45" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45">
         <f>COUNTIF(D45:D47,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H45">
         <f>COUNTIF(D45:D47,"Parcialmente")</f>
@@ -10956,7 +11004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15">
+    <row r="46" spans="1:10" ht="14.4">
       <c r="A46" s="31"/>
       <c r="B46" s="5">
         <v>31</v>
@@ -10964,11 +11012,13 @@
       <c r="C46" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:10" ht="30">
+    <row r="47" spans="1:10" ht="28.8">
       <c r="A47" s="31"/>
       <c r="B47" s="5">
         <v>32</v>
@@ -10976,11 +11026,13 @@
       <c r="C47" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:10" ht="15">
+    <row r="48" spans="1:10" ht="14.4">
       <c r="A48" s="31"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10" t="s">
@@ -10990,7 +11042,7 @@
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
     </row>
-    <row r="49" spans="1:10" ht="30">
+    <row r="49" spans="1:10" ht="28.8">
       <c r="A49" s="31"/>
       <c r="B49" s="5">
         <v>33</v>
@@ -10998,7 +11050,9 @@
       <c r="C49" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49">
@@ -11015,10 +11069,10 @@
       </c>
       <c r="J49">
         <f>COUNTIF(D49:D51,"NA")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="14.4">
       <c r="A50" s="31"/>
       <c r="B50" s="5">
         <v>34</v>
@@ -11026,11 +11080,13 @@
       <c r="C50" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:10" ht="15">
+    <row r="51" spans="1:10" ht="14.4">
       <c r="A51" s="31"/>
       <c r="B51" s="5">
         <v>35</v>
@@ -11038,51 +11094,53 @@
       <c r="C51" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="60" spans="1:10" ht="15">
+    <row r="60" spans="1:10" ht="14.4">
       <c r="B60"/>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:10" ht="15">
+    <row r="61" spans="1:10" ht="14.4">
       <c r="B61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:10" ht="15">
+    <row r="62" spans="1:10" ht="14.4">
       <c r="B62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:10" ht="15">
+    <row r="63" spans="1:10" ht="14.4">
       <c r="B63"/>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:10" ht="15">
+    <row r="64" spans="1:10" ht="14.4">
       <c r="B64"/>
       <c r="C64"/>
     </row>
-    <row r="65" spans="2:3" ht="15">
+    <row r="65" spans="2:3" ht="14.4">
       <c r="B65"/>
       <c r="C65"/>
     </row>
-    <row r="66" spans="2:3" ht="15">
+    <row r="66" spans="2:3" ht="14.4">
       <c r="B66"/>
       <c r="C66"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11105,14 +11163,14 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="71.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
     <col min="7" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11141,7 +11199,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5" thickBot="1">
+    <row r="3" spans="1:10" ht="16.2" thickBot="1">
       <c r="A3" s="35" t="s">
         <v>26</v>
       </c>
@@ -11153,7 +11211,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="39"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" ht="14.4">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -11185,7 +11243,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="28.8">
       <c r="A6" s="33"/>
       <c r="B6" s="5">
         <v>1</v>
@@ -11213,7 +11271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" ht="14.4">
       <c r="A7" s="33"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
@@ -11223,7 +11281,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A8" s="33"/>
       <c r="B8" s="5">
         <v>2</v>
@@ -11251,7 +11309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10" ht="14.4">
       <c r="A9" s="33"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
@@ -11261,7 +11319,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="45">
+    <row r="10" spans="1:10" ht="43.2">
       <c r="A10" s="33"/>
       <c r="B10" s="5">
         <v>3</v>
@@ -11289,7 +11347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30">
+    <row r="11" spans="1:10" ht="28.8">
       <c r="A11" s="33"/>
       <c r="B11" s="5">
         <v>4</v>
@@ -11313,7 +11371,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10" ht="14.4">
       <c r="A13" s="33"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
@@ -11323,7 +11381,7 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" ht="14.4">
       <c r="A14" s="33"/>
       <c r="B14" s="5">
         <v>6</v>
@@ -11351,7 +11409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" ht="14.4">
       <c r="A15" s="33"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
@@ -11361,7 +11419,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="30">
+    <row r="16" spans="1:10" ht="28.8">
       <c r="A16" s="33"/>
       <c r="B16" s="5">
         <v>7</v>
@@ -11401,7 +11459,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10" ht="14.4">
       <c r="A18" s="33"/>
       <c r="B18" s="5">
         <v>8</v>
@@ -11441,7 +11499,7 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:10" ht="30">
+    <row r="20" spans="1:10" ht="14.4">
       <c r="A20" s="33"/>
       <c r="B20" s="5">
         <v>9</v>
@@ -11469,7 +11527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15">
+    <row r="21" spans="1:10" ht="14.4">
       <c r="A21" s="33"/>
       <c r="B21" s="5">
         <v>10</v>
@@ -11481,7 +11539,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="30">
+    <row r="22" spans="1:10" ht="14.4">
       <c r="A22" s="33"/>
       <c r="B22" s="5">
         <v>11</v>
@@ -11493,7 +11551,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10" ht="14.4">
       <c r="A23" s="33"/>
       <c r="B23" s="5">
         <v>12</v>
@@ -11505,7 +11563,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="15">
+    <row r="24" spans="1:10" ht="14.4">
       <c r="A24" s="36"/>
       <c r="B24" s="5">
         <v>13</v>
@@ -11517,7 +11575,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10" ht="14.4">
       <c r="A25" s="32" t="s">
         <v>20</v>
       </c>
@@ -11529,7 +11587,7 @@
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:10" ht="15">
+    <row r="26" spans="1:10" ht="14.4">
       <c r="A26" s="33"/>
       <c r="B26" s="5">
         <v>14</v>
@@ -11557,7 +11615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10" ht="14.4">
       <c r="A27" s="33"/>
       <c r="B27" s="5">
         <v>15</v>
@@ -11569,7 +11627,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="15">
+    <row r="28" spans="1:10" ht="14.4">
       <c r="A28" s="36"/>
       <c r="B28" s="5">
         <v>16</v>
@@ -11593,7 +11651,7 @@
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="30" spans="1:10" s="1" customFormat="1" ht="28.8">
       <c r="A30" s="33"/>
       <c r="B30" s="23">
         <v>24</v>
@@ -11621,7 +11679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" ht="45">
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="43.2">
       <c r="A31" s="33"/>
       <c r="B31" s="5">
         <v>25</v>
@@ -11633,7 +11691,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="15">
+    <row r="32" spans="1:10" ht="14.4">
       <c r="A32" s="33"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10" t="s">
@@ -11643,7 +11701,7 @@
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:10" ht="30">
+    <row r="33" spans="1:10" ht="28.8">
       <c r="A33" s="33"/>
       <c r="B33" s="23">
         <v>26</v>
@@ -11671,7 +11729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15">
+    <row r="34" spans="1:10" ht="14.4">
       <c r="A34" s="36"/>
       <c r="B34" s="5">
         <v>27</v>
@@ -11683,7 +11741,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="15">
+    <row r="35" spans="1:10" ht="14.4">
       <c r="A35" s="42" t="s">
         <v>11</v>
       </c>
@@ -11695,7 +11753,7 @@
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="1:10" ht="30">
+    <row r="36" spans="1:10" ht="28.8">
       <c r="A36" s="42"/>
       <c r="B36" s="5">
         <v>19</v>
@@ -11723,7 +11781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="45">
+    <row r="37" spans="1:10" ht="43.2">
       <c r="A37" s="42"/>
       <c r="B37" s="5">
         <v>20</v>
@@ -11735,7 +11793,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="30">
+    <row r="38" spans="1:10" ht="14.4">
       <c r="A38" s="42"/>
       <c r="B38" s="5">
         <v>21</v>
@@ -11747,7 +11805,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="15">
+    <row r="39" spans="1:10" ht="14.4">
       <c r="A39" s="42"/>
       <c r="B39" s="5">
         <v>22</v>
@@ -11759,7 +11817,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="15">
+    <row r="40" spans="1:10" ht="14.4">
       <c r="A40" s="42"/>
       <c r="B40" s="5">
         <v>23</v>
@@ -11771,7 +11829,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="30">
+    <row r="41" spans="1:10" ht="14.4">
       <c r="A41" s="42"/>
       <c r="B41" s="5">
         <v>24</v>
@@ -11783,7 +11841,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:10" ht="15">
+    <row r="42" spans="1:10" ht="14.4">
       <c r="A42" s="42"/>
       <c r="B42" s="5">
         <v>25</v>
@@ -11807,7 +11865,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="1:10" ht="30">
+    <row r="44" spans="1:10" ht="28.8">
       <c r="A44" s="31"/>
       <c r="B44" s="5">
         <v>26</v>
@@ -11835,7 +11893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15">
+    <row r="45" spans="1:10" ht="14.4">
       <c r="A45" s="31"/>
       <c r="B45" s="5">
         <v>27</v>
@@ -11847,7 +11905,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:10" ht="30">
+    <row r="46" spans="1:10" ht="28.8">
       <c r="A46" s="31"/>
       <c r="B46" s="5">
         <v>28</v>
@@ -11859,7 +11917,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:10" ht="15">
+    <row r="47" spans="1:10" ht="14.4">
       <c r="A47" s="31"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
@@ -11869,7 +11927,7 @@
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="1:10" ht="30">
+    <row r="48" spans="1:10" ht="28.8">
       <c r="A48" s="31"/>
       <c r="B48" s="5">
         <v>29</v>
@@ -11897,7 +11955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15">
+    <row r="49" spans="1:6" ht="14.4">
       <c r="A49" s="31"/>
       <c r="B49" s="5">
         <v>30</v>
@@ -11909,7 +11967,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" ht="15">
+    <row r="50" spans="1:6" ht="14.4">
       <c r="A50" s="31"/>
       <c r="B50" s="5">
         <v>31</v>
@@ -11921,36 +11979,41 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="59" spans="1:6" ht="15">
+    <row r="59" spans="1:6" ht="14.4">
       <c r="B59"/>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:6" ht="15">
+    <row r="60" spans="1:6" ht="14.4">
       <c r="B60"/>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:6" ht="15">
+    <row r="61" spans="1:6" ht="14.4">
       <c r="B61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:6" ht="15">
+    <row r="62" spans="1:6" ht="14.4">
       <c r="B62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:6" ht="15">
+    <row r="63" spans="1:6" ht="14.4">
       <c r="B63"/>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:6" ht="15">
+    <row r="64" spans="1:6" ht="14.4">
       <c r="B64"/>
       <c r="C64"/>
     </row>
-    <row r="65" spans="2:3" ht="15">
+    <row r="65" spans="2:3" ht="14.4">
       <c r="B65"/>
       <c r="C65"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -11958,11 +12021,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
mudanças documentos para fase de implantação
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E35722-E0F8-4B22-9021-A936A0E0A261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A926703-60E2-43EA-947A-72D078D78A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="2400" windowWidth="21600" windowHeight="11205" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,7 +1644,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0909090909090908</c:v>
+                  <c:v>1.0869565217391304</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3355,7 +3355,7 @@
                   <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -3712,7 +3712,7 @@
                   <c:v>0.42857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="B5" s="20">
         <f>'Ver-Construção1'!$F$2</f>
-        <v>1.0909090909090908</v>
+        <v>1.0869565217391304</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -8248,7 +8248,7 @@
       </c>
       <c r="B32" s="28">
         <f>('Ver-Construção1'!$G$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C32" s="28">
         <f>('Ver-Construção1'!$H$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
@@ -8260,7 +8260,7 @@
       </c>
       <c r="E32" s="28">
         <f>('Ver-Construção1'!$J$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M32" t="s">
         <v>8</v>
@@ -10215,7 +10215,7 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -10251,7 +10251,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D51,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>1.0909090909090908</v>
+        <v>1.0869565217391304</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1">
@@ -10877,7 +10877,7 @@
       <c r="F38" s="8"/>
       <c r="G38">
         <f>COUNTIF(D38:D43,"Sim")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H38">
         <f>COUNTIF(D38:D43,"Parcialmente")</f>
@@ -10889,7 +10889,7 @@
       </c>
       <c r="J38">
         <f>COUNTIF(D38:D43,"NA")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45">
@@ -10915,7 +10915,7 @@
         <v>65</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -11130,17 +11130,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11160,7 +11160,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -12015,6 +12015,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -12022,11 +12027,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
Update Checklist de Verificação e Planilia de Planejamento
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
+++ b/Gerenciamento de Projeto/AGP - Checklist Verificacao de Projeto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A926703-60E2-43EA-947A-72D078D78A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C29D62-56C7-4DCE-8A1F-28861DBBAFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2400" windowWidth="21600" windowHeight="11205" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="2400" windowWidth="21600" windowHeight="11205" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -713,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="128">
   <si>
     <t>Ambiente</t>
   </si>
@@ -4085,34 +4085,34 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -4460,11 +4460,11 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4475,7 +4475,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4490,7 +4490,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8067,7 +8067,7 @@
       </c>
       <c r="N27" s="28">
         <f>('Ver-Transição1'!$G$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="O27" s="28">
         <f>('Ver-Transição1'!$H$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
@@ -8079,7 +8079,7 @@
       </c>
       <c r="Q27" s="28">
         <f>('Ver-Transição1'!$J$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -8105,21 +8105,21 @@
       <c r="M28" t="s">
         <v>4</v>
       </c>
-      <c r="N28" s="28" t="e">
+      <c r="N28" s="28">
         <f>('Ver-Transição1'!$G$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="O28" s="28">
         <f>('Ver-Transição1'!$H$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P28" s="28">
         <f>('Ver-Transição1'!$I$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="28">
         <f>('Ver-Transição1'!$J$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -8145,21 +8145,21 @@
       <c r="M29" t="s">
         <v>36</v>
       </c>
-      <c r="N29" s="28" t="e">
+      <c r="N29" s="28">
         <f>('Ver-Transição1'!$G$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O29" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="O29" s="28">
         <f>('Ver-Transição1'!$H$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P29" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P29" s="28">
         <f>('Ver-Transição1'!$I$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q29" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="28">
         <f>('Ver-Transição1'!$J$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -8185,21 +8185,21 @@
       <c r="M30" t="s">
         <v>5</v>
       </c>
-      <c r="N30" s="28" t="e">
+      <c r="N30" s="28">
         <f>('Ver-Transição1'!$G$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O30" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="O30" s="28">
         <f>('Ver-Transição1'!$H$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P30" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P30" s="28">
         <f>('Ver-Transição1'!$I$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q30" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="28">
         <f>('Ver-Transição1'!$J$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -8225,21 +8225,21 @@
       <c r="M31" t="s">
         <v>6</v>
       </c>
-      <c r="N31" s="28" t="e">
+      <c r="N31" s="28">
         <f>('Ver-Transição1'!$G$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O31" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="O31" s="28">
         <f>('Ver-Transição1'!$H$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P31" s="28">
         <f>('Ver-Transição1'!$I$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q31" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="28">
         <f>('Ver-Transição1'!$J$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -8265,21 +8265,21 @@
       <c r="M32" t="s">
         <v>8</v>
       </c>
-      <c r="N32" s="28" t="e">
+      <c r="N32" s="28">
         <f>('Ver-Transição1'!$G$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O32" s="28" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O32" s="28">
         <f>('Ver-Transição1'!$H$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P32" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P32" s="28">
         <f>('Ver-Transição1'!$I$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q32" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="28">
         <f>('Ver-Transição1'!$J$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -8305,21 +8305,21 @@
       <c r="M33" t="s">
         <v>9</v>
       </c>
-      <c r="N33" s="28" t="e">
+      <c r="N33" s="28">
         <f>('Ver-Transição1'!$G$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O33" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="O33" s="28">
         <f>('Ver-Transição1'!$H$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P33" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P33" s="28">
         <f>('Ver-Transição1'!$I$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q33" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="28">
         <f>('Ver-Transição1'!$J$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -8345,84 +8345,84 @@
       <c r="M34" t="s">
         <v>10</v>
       </c>
-      <c r="N34" s="27" t="e">
+      <c r="N34" s="27">
         <f>('Ver-Transição1'!$G$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O34" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="O34" s="28">
         <f>('Ver-Transição1'!$H$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P34" s="28">
         <f>('Ver-Transição1'!$I$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q34" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="28">
         <f>('Ver-Transição1'!$J$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="M35" t="s">
         <v>13</v>
       </c>
-      <c r="N35" s="28" t="e">
+      <c r="N35" s="28">
         <f>('Ver-Transição1'!$G$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O35" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="O35" s="28">
         <f>('Ver-Transição1'!$H$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P35" s="28">
         <f>('Ver-Transição1'!$I$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q35" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="28">
         <f>('Ver-Transição1'!$J$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="M36" t="s">
         <v>70</v>
       </c>
-      <c r="N36" s="28" t="e">
+      <c r="N36" s="28">
         <f>('Ver-Transição1'!$G$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O36" s="28" t="e">
+        <v>1</v>
+      </c>
+      <c r="O36" s="28">
         <f>('Ver-Transição1'!$H$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P36" s="28">
         <f>('Ver-Transição1'!$I$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q36" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="28">
         <f>('Ver-Transição1'!$J$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:17">
       <c r="M37" t="s">
         <v>15</v>
       </c>
-      <c r="N37" s="28" t="e">
+      <c r="N37" s="28">
         <f>('Ver-Transição1'!$G$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O37" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="O37" s="28">
         <f>('Ver-Transição1'!$H$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="P37" s="28">
         <f>('Ver-Transição1'!$I$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q37" s="28" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="28">
         <f>('Ver-Transição1'!$J$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8438,7 +8438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -9354,7 +9354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="B24" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -10214,7 +10214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C39" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -11130,17 +11130,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D20 D17 D22 D48 D44 D37" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11159,8 +11159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -11332,13 +11332,13 @@
         <v>71</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10">
         <f>COUNTIF(D10:D12,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <f>COUNTIF(D10:D12,"Parcialmente")</f>
@@ -11361,7 +11361,9 @@
       <c r="C11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
@@ -11373,7 +11375,9 @@
       <c r="C12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -11395,7 +11399,9 @@
       <c r="C14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14">
@@ -11412,7 +11418,7 @@
       </c>
       <c r="J14">
         <f>COUNTIF(D14,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15">
@@ -11433,12 +11439,14 @@
       <c r="C16" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
         <f>COUNTIF(D16,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <f>COUNTIF(D16,"Parcialmente")</f>
@@ -11473,12 +11481,14 @@
       <c r="C18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18">
         <f>COUNTIF(D18,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <f>COUNTIF(D18,"Parcialmente")</f>
@@ -11513,12 +11523,14 @@
       <c r="C20" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20">
         <f>COUNTIF(D20:D24,"Sim")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20">
         <f>COUNTIF(D20:D24,"Parcialmente")</f>
@@ -11541,7 +11553,9 @@
       <c r="C21" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -11553,7 +11567,9 @@
       <c r="C22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
@@ -11565,7 +11581,9 @@
       <c r="C23" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
@@ -11577,7 +11595,9 @@
       <c r="C24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
@@ -11601,12 +11621,14 @@
       <c r="C26" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26">
         <f>COUNTIF(D26:D28,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f>COUNTIF(D26:D28,"Parcialmente")</f>
@@ -11618,7 +11640,7 @@
       </c>
       <c r="J26">
         <f>COUNTIF(D26:D28,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30">
@@ -11629,7 +11651,9 @@
       <c r="C27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
@@ -11641,7 +11665,9 @@
       <c r="C28" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
@@ -11665,12 +11691,14 @@
       <c r="C30" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30">
         <f>COUNTIF(D30:D31,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30">
         <f>COUNTIF(D30:D31,"Parcialmente")</f>
@@ -11693,7 +11721,9 @@
       <c r="C31" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -11715,12 +11745,14 @@
       <c r="C33" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33">
         <f>COUNTIF(D33:D34,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33">
         <f>COUNTIF(D33:D34,"Parcialmente")</f>
@@ -11743,7 +11775,9 @@
       <c r="C34" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -11767,12 +11801,14 @@
       <c r="C36" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36">
         <f>COUNTIF(D36:D42,"Sim")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H36">
         <f>COUNTIF(D36:D42,"Parcialmente")</f>
@@ -11795,7 +11831,9 @@
       <c r="C37" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
@@ -11807,7 +11845,9 @@
       <c r="C38" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -11819,7 +11859,9 @@
       <c r="C39" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
@@ -11831,7 +11873,9 @@
       <c r="C40" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
@@ -11843,7 +11887,9 @@
       <c r="C41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
@@ -11855,7 +11901,9 @@
       <c r="C42" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
@@ -11879,12 +11927,14 @@
       <c r="C44" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44">
         <f>COUNTIF(D44:D46,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H44">
         <f>COUNTIF(D44:D46,"Parcialmente")</f>
@@ -11907,7 +11957,9 @@
       <c r="C45" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
@@ -11919,7 +11971,9 @@
       <c r="C46" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
@@ -11941,7 +11995,9 @@
       <c r="C48" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48">
@@ -11958,7 +12014,7 @@
       </c>
       <c r="J48">
         <f>COUNTIF(D48:D50,"NA")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15">
@@ -11969,7 +12025,9 @@
       <c r="C49" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
@@ -11981,7 +12039,9 @@
       <c r="C50" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
@@ -12015,11 +12075,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -12027,6 +12082,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29 D19 D17 D25 D47 D43 D35 D32" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>